<commit_message>
Crear primera version de output contable con BTs
</commit_message>
<xml_diff>
--- a/prototipo_pcr/inputs/nomenclatura.xlsx
+++ b/prototipo_pcr/inputs/nomenclatura.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://suramericana.sharepoint.com/sites/TraNIFF/Shared Documents/féniX/01 IFRS17/02 Entregables Procesos/05 Reservas/03 PCR CP/03 Tecnología/01 Prototipo/prototipo_pcr/inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebatoec/Library/CloudStorage/OneDrive-SharedLibraries-SegurosSuramericana,S.A/Proyecto féniX - féniX/01 IFRS17/02 Entregables Procesos/05 Reservas/03 PCR CP/03 Tecnología/01 Prototipo/prototipo_pcr/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="14_{64B8E926-A252-8F4A-A82F-9CE870E39367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8EF1A9CB-B10D-3643-BF9F-9ABB7A4FCFAC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F15FDB-F165-B749-B3CF-41A5F3C35FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1820" windowWidth="27240" windowHeight="16200" xr2:uid="{B6BBB8B8-7677-D84C-AD85-43B73374E2C3}"/>
+    <workbookView xWindow="1900" yWindow="1140" windowWidth="27240" windowHeight="16200" activeTab="1" xr2:uid="{B6BBB8B8-7677-D84C-AD85-43B73374E2C3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="V1" sheetId="1" r:id="rId1"/>
+    <sheet name="V2" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029" iterate="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="351">
   <si>
     <t>Campo</t>
   </si>
@@ -284,9 +285,6 @@
     <t>Gto de liquidación</t>
   </si>
   <si>
-    <t>RA</t>
-  </si>
-  <si>
     <t>Deterioro</t>
   </si>
   <si>
@@ -398,9 +396,6 @@
     <t>Aviso</t>
   </si>
   <si>
-    <t>MAT_CP</t>
-  </si>
-  <si>
     <t>PCR_LP</t>
   </si>
   <si>
@@ -413,27 +408,12 @@
     <t>CAM</t>
   </si>
   <si>
-    <t>NP primas = costo contrato</t>
-  </si>
-  <si>
     <t>Comentarios</t>
   </si>
   <si>
-    <t>qué es</t>
-  </si>
-  <si>
-    <t>TMT</t>
-  </si>
-  <si>
     <t>comercial para diferenciar de posible interpretación de VDT</t>
   </si>
   <si>
-    <t>podemos incluir esta diferenciacion aquí o en concepto?</t>
-  </si>
-  <si>
-    <t>Factor Terremoto</t>
-  </si>
-  <si>
     <t>GNT</t>
   </si>
   <si>
@@ -443,9 +423,6 @@
     <t>DAC</t>
   </si>
   <si>
-    <t>podemos incluir esta diferenciacion aquí?</t>
-  </si>
-  <si>
     <t>01</t>
   </si>
   <si>
@@ -461,9 +438,6 @@
     <t>reaseguro</t>
   </si>
   <si>
-    <t>produccion</t>
-  </si>
-  <si>
     <t>fluctuacion</t>
   </si>
   <si>
@@ -479,12 +453,6 @@
     <t>no_aplica</t>
   </si>
   <si>
-    <t>se refiere a descuento VDT o descuento comercial? Dcto comercial ya está en concepto, el movimiento no debería clasificarse como descuento</t>
-  </si>
-  <si>
-    <t>ya hay conceptos de cartera, aquí no debería ser saldo o movimiento?</t>
-  </si>
-  <si>
     <t>anio_anterior</t>
   </si>
   <si>
@@ -510,13 +478,625 @@
   </si>
   <si>
     <t>ext</t>
+  </si>
+  <si>
+    <t>Vida / Gen se separa</t>
+  </si>
+  <si>
+    <t>se refiere a descuento VDT, NO descuento comercial</t>
+  </si>
+  <si>
+    <t>Movimiento Cartera</t>
+  </si>
+  <si>
+    <t>Recoge delta de saldos vs periodo anterior</t>
+  </si>
+  <si>
+    <t>Ajuste de Riesgo</t>
+  </si>
+  <si>
+    <t>ADR</t>
+  </si>
+  <si>
+    <t>Risk Adjustment (antes RA)</t>
+  </si>
+  <si>
+    <t>Para reaseguro NP Autom primas = costo contrato</t>
+  </si>
+  <si>
+    <t>Conectar con la BT de terremoto</t>
+  </si>
+  <si>
+    <t>Terremoto</t>
+  </si>
+  <si>
+    <t>Se usa en largo plazo como saldo inicial de reserva bajo NIIF4</t>
+  </si>
+  <si>
+    <t>Incluir</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>prima</t>
+  </si>
+  <si>
+    <t>gasto_exp_comisiones</t>
+  </si>
+  <si>
+    <t>gasto_exp_otros</t>
+  </si>
+  <si>
+    <t>descuento_comercial</t>
+  </si>
+  <si>
+    <t>terremoto_nota_tecnica</t>
+  </si>
+  <si>
+    <t>camara_soat</t>
+  </si>
+  <si>
+    <t>onerosidad</t>
+  </si>
+  <si>
+    <t>comision_cesion</t>
+  </si>
+  <si>
+    <t>se refiere a descuento VP, NO descuento comercial</t>
+  </si>
+  <si>
+    <t>Variación de tasas PYG</t>
+  </si>
+  <si>
+    <t>VTP</t>
+  </si>
+  <si>
+    <t>Variación de tasas ORI</t>
+  </si>
+  <si>
+    <t>VTO</t>
+  </si>
+  <si>
+    <t>MO</t>
+  </si>
+  <si>
+    <t>Alianza Bancolombia</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>alianza banco</t>
+  </si>
+  <si>
+    <t>no aplica</t>
+  </si>
+  <si>
+    <t>bel</t>
+  </si>
+  <si>
+    <t>gto de liquidación</t>
+  </si>
+  <si>
+    <t>ajuste de riesgo</t>
+  </si>
+  <si>
+    <t>deterioro</t>
+  </si>
+  <si>
+    <t>fondo ahorro</t>
+  </si>
+  <si>
+    <t>contable reclasificación</t>
+  </si>
+  <si>
+    <t>csm</t>
+  </si>
+  <si>
+    <t>niif4</t>
+  </si>
+  <si>
+    <t>reserva</t>
+  </si>
+  <si>
+    <t>cartera</t>
+  </si>
+  <si>
+    <t>comercial para diferenciar de posible interpretación de VP</t>
+  </si>
+  <si>
+    <t>dac</t>
+  </si>
+  <si>
+    <t>Matemática</t>
+  </si>
+  <si>
+    <t>MAT</t>
+  </si>
+  <si>
+    <t>Etapa</t>
+  </si>
+  <si>
+    <t>Reconocimiento Inicial</t>
+  </si>
+  <si>
+    <t>reconocimiento inicial</t>
+  </si>
+  <si>
+    <t>transición</t>
+  </si>
+  <si>
+    <t>Acreditación de intereses</t>
+  </si>
+  <si>
+    <t>acreditación de intereses</t>
+  </si>
+  <si>
+    <t>Primas Emt netas de GA</t>
+  </si>
+  <si>
+    <t>primas emt netas de ga</t>
+  </si>
+  <si>
+    <t>Ajuste Experiencia</t>
+  </si>
+  <si>
+    <t>ajuste experiencia</t>
+  </si>
+  <si>
+    <t>Reconocimiento de Ingresos</t>
+  </si>
+  <si>
+    <t>reconocimiento de ingresos</t>
+  </si>
+  <si>
+    <t>ORI -Vción hipótesis Fras</t>
+  </si>
+  <si>
+    <t>ori -vción hipótesis fras</t>
+  </si>
+  <si>
+    <t>ORI-Vción tasa de interés</t>
+  </si>
+  <si>
+    <t>ori-vción tasa de interés</t>
+  </si>
+  <si>
+    <t>Vción hipótesis Fras</t>
+  </si>
+  <si>
+    <t>vción hipótesis fras</t>
+  </si>
+  <si>
+    <t>Ef.vción que no afecta CSM</t>
+  </si>
+  <si>
+    <t>ef.vción que no afecta csm</t>
+  </si>
+  <si>
+    <t>Componente de Inv no PU</t>
+  </si>
+  <si>
+    <t>componente de inv no pu</t>
+  </si>
+  <si>
+    <t>Pago Comp de Inv no PU</t>
+  </si>
+  <si>
+    <t>pago comp de inv no pu</t>
+  </si>
+  <si>
+    <t>Componente de Inv PU FA</t>
+  </si>
+  <si>
+    <t>componente de inv pu fa</t>
+  </si>
+  <si>
+    <t>Pago Comp de Inv PU FA</t>
+  </si>
+  <si>
+    <t>pago comp de inv pu fa</t>
+  </si>
+  <si>
+    <t>Ajuste de Expe. PU FA</t>
+  </si>
+  <si>
+    <t>ajuste de expe. pu fa</t>
+  </si>
+  <si>
+    <t>Transición LIC</t>
+  </si>
+  <si>
+    <t>transición lic</t>
+  </si>
+  <si>
+    <t>Reconocimiento Inicial_O</t>
+  </si>
+  <si>
+    <t>reconocimiento inicial_o</t>
+  </si>
+  <si>
+    <t>Transición_O</t>
+  </si>
+  <si>
+    <t>transición_o</t>
+  </si>
+  <si>
+    <t>Ajuste Experiencia_O</t>
+  </si>
+  <si>
+    <t>ajuste experiencia_o</t>
+  </si>
+  <si>
+    <t>Ajuste Exp. LC a CSM</t>
+  </si>
+  <si>
+    <t>ajuste exp. lc a csm</t>
+  </si>
+  <si>
+    <t>Aj.Exp.LCaCSM d.1año</t>
+  </si>
+  <si>
+    <t>aj.exp.lcacsm d.1año</t>
+  </si>
+  <si>
+    <t>Ajuste Exp. CSM a LC</t>
+  </si>
+  <si>
+    <t>ajuste exp. csm a lc</t>
+  </si>
+  <si>
+    <t>Revers.Onerosidad</t>
+  </si>
+  <si>
+    <t>revers.onerosidad</t>
+  </si>
+  <si>
+    <t>Amort.Gt.Adquisición</t>
+  </si>
+  <si>
+    <t>amort.gt.adquisición</t>
+  </si>
+  <si>
+    <t>Movimiento DAC</t>
+  </si>
+  <si>
+    <t>movimiento dac</t>
+  </si>
+  <si>
+    <t>Ajuste Diferencia en Cambio</t>
+  </si>
+  <si>
+    <t>ajuste diferencia en cambio</t>
+  </si>
+  <si>
+    <t>Auxiliar nombre flujo</t>
+  </si>
+  <si>
+    <t>PCR - Primas</t>
+  </si>
+  <si>
+    <t>pcr - primas</t>
+  </si>
+  <si>
+    <t>PCR - BEL - Gastos de Adquisición comisiones</t>
+  </si>
+  <si>
+    <t>pcr - bel - gastos de adquisición comisiones</t>
+  </si>
+  <si>
+    <t>PCR - BEL Otros gastos de Adquisición</t>
+  </si>
+  <si>
+    <t>pcr - bel otros gastos de adquisición</t>
+  </si>
+  <si>
+    <t>PCR - BEL - Siniestralidad Mortalidad</t>
+  </si>
+  <si>
+    <t>pcr - bel - siniestralidad mortalidad</t>
+  </si>
+  <si>
+    <t>PCR - BEL - Siniestralidad Sobrevivencia</t>
+  </si>
+  <si>
+    <t>pcr - bel - siniestralidad sobrevivencia</t>
+  </si>
+  <si>
+    <t>PCR - BEL - Siniestralidad Exoneración de prima</t>
+  </si>
+  <si>
+    <t>pcr - bel - siniestralidad exoneración de prima</t>
+  </si>
+  <si>
+    <t>PCR - BEL - Siniestralidad Otras opcionalidades</t>
+  </si>
+  <si>
+    <t>pcr - bel - siniestralidad otras opcionalidades</t>
+  </si>
+  <si>
+    <t>PCR - BEL - Siniestralidad Rescates</t>
+  </si>
+  <si>
+    <t>pcr - bel - siniestralidad rescates</t>
+  </si>
+  <si>
+    <t>PCR - BEL - Siniestralidad PU inv VA</t>
+  </si>
+  <si>
+    <t>pcr - bel - siniestralidad pu inv va</t>
+  </si>
+  <si>
+    <t>PCR - BEL - Siniestralidad PU tecnica VA</t>
+  </si>
+  <si>
+    <t>pcr - bel - siniestralidad pu tecnica va</t>
+  </si>
+  <si>
+    <t>PCR - BEL - Siniestralidad PU tecnica FA</t>
+  </si>
+  <si>
+    <t>pcr - bel - siniestralidad pu tecnica fa</t>
+  </si>
+  <si>
+    <t>PCR - BEL - Siniestralidad PU Rentas</t>
+  </si>
+  <si>
+    <t>pcr - bel - siniestralidad pu rentas</t>
+  </si>
+  <si>
+    <t>PCR - BEL - Siniestralidad Agregada</t>
+  </si>
+  <si>
+    <t>pcr - bel - siniestralidad agregada</t>
+  </si>
+  <si>
+    <t>PCR - BEL - Siniestralidad CI AB</t>
+  </si>
+  <si>
+    <t>pcr - bel - siniestralidad ci ab</t>
+  </si>
+  <si>
+    <t>PCR - BEL - Siniestralidad CI PU (INVFA)</t>
+  </si>
+  <si>
+    <t>pcr - bel - siniestralidad ci pu (invfa)</t>
+  </si>
+  <si>
+    <t>PCR - BEL - Otros Gastos atribuibles</t>
+  </si>
+  <si>
+    <t>pcr - bel - otros gastos atribuibles</t>
+  </si>
+  <si>
+    <t>PCR - RA</t>
+  </si>
+  <si>
+    <t>pcr - ra</t>
+  </si>
+  <si>
+    <t>Cuenta puente Reservas IFRS4</t>
+  </si>
+  <si>
+    <t>cuenta puente reservas ifrs4</t>
+  </si>
+  <si>
+    <t>PCR - CSM</t>
+  </si>
+  <si>
+    <t>pcr - csm</t>
+  </si>
+  <si>
+    <t>Cuenta puente cuentas por pagar</t>
+  </si>
+  <si>
+    <t>cuenta puente cuentas por pagar</t>
+  </si>
+  <si>
+    <t>Variación de tasas e hipótesis financieras - PCR BEL</t>
+  </si>
+  <si>
+    <t>variación de tasas e hipótesis financieras - pcr bel</t>
+  </si>
+  <si>
+    <t>PRI - BEL Siniestralidad Agregada</t>
+  </si>
+  <si>
+    <t>pri - bel siniestralidad agregada</t>
+  </si>
+  <si>
+    <t>PRI - BEL Otros gastos atribuibles</t>
+  </si>
+  <si>
+    <t>pri - bel otros gastos atribuibles</t>
+  </si>
+  <si>
+    <t>PRI - RA</t>
+  </si>
+  <si>
+    <t>pri - ra</t>
+  </si>
+  <si>
+    <t>Ajuste de Experiencia a LC</t>
+  </si>
+  <si>
+    <t>ajuste de experiencia a lc</t>
+  </si>
+  <si>
+    <t>Cuenta Transito</t>
+  </si>
+  <si>
+    <t>cuenta transito</t>
+  </si>
+  <si>
+    <t>Reversión Loss Component RA</t>
+  </si>
+  <si>
+    <t>reversión loss component ra</t>
+  </si>
+  <si>
+    <t>Reversión Loss Component BEL</t>
+  </si>
+  <si>
+    <t>reversión loss component bel</t>
+  </si>
+  <si>
+    <t>Reversión Loss Component G. Adquisición</t>
+  </si>
+  <si>
+    <t>reversión loss component g. adquisición</t>
+  </si>
+  <si>
+    <t>Amort Gastos de Adquisición Comisiones Bruto</t>
+  </si>
+  <si>
+    <t>amort gastos de adquisición comisiones bruto</t>
+  </si>
+  <si>
+    <t>Recuperación Gastos de Adquisición Comisiones Bruto</t>
+  </si>
+  <si>
+    <t>recuperación gastos de adquisición comisiones bruto</t>
+  </si>
+  <si>
+    <t>Amort Otros Gastos de Adquisición Bruto</t>
+  </si>
+  <si>
+    <t>amort otros gastos de adquisición bruto</t>
+  </si>
+  <si>
+    <t>Recuperación Otros Gastos de Adquisición Bruto</t>
+  </si>
+  <si>
+    <t>recuperación otros gastos de adquisición bruto</t>
+  </si>
+  <si>
+    <t>CIND Esperado (Componente de Inversión No Distinto)</t>
+  </si>
+  <si>
+    <t>cind esperado (componente de inversión no distinto)</t>
+  </si>
+  <si>
+    <t>PRI - Primas</t>
+  </si>
+  <si>
+    <t>pri - primas</t>
+  </si>
+  <si>
+    <t>PRI - BEL Gastos de Adquisición comisiones</t>
+  </si>
+  <si>
+    <t>pri - bel gastos de adquisición comisiones</t>
+  </si>
+  <si>
+    <t>PRI - BEL Otros gastos de Adquisición</t>
+  </si>
+  <si>
+    <t>pri - bel otros gastos de adquisición</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRI - BEL Siniestralidad Mortalidad </t>
+  </si>
+  <si>
+    <t>pri - bel siniestralidad mortalidad</t>
+  </si>
+  <si>
+    <t>PRI - BEL Siniestralidad Sobrevivencia</t>
+  </si>
+  <si>
+    <t>pri - bel siniestralidad sobrevivencia</t>
+  </si>
+  <si>
+    <t>PRI - BEL Siniestralidad Otras Opcionalidades</t>
+  </si>
+  <si>
+    <t>pri - bel siniestralidad otras opcionalidades</t>
+  </si>
+  <si>
+    <t>PRI - BEL Siniestralidad PU Rentas</t>
+  </si>
+  <si>
+    <t>pri - bel siniestralidad pu rentas</t>
+  </si>
+  <si>
+    <t>Comisiones No Exigible</t>
+  </si>
+  <si>
+    <t>comisiones no exigible</t>
+  </si>
+  <si>
+    <t>Otro No Exigible</t>
+  </si>
+  <si>
+    <t>otro no exigible</t>
+  </si>
+  <si>
+    <t>Comisiones Exigible</t>
+  </si>
+  <si>
+    <t>comisiones exigible</t>
+  </si>
+  <si>
+    <t>Otro Exigible</t>
+  </si>
+  <si>
+    <t>otro exigible</t>
+  </si>
+  <si>
+    <t>Gasto Financiero</t>
+  </si>
+  <si>
+    <t>gasto financiero</t>
+  </si>
+  <si>
+    <t>Acreditación Intereses</t>
+  </si>
+  <si>
+    <t>acreditación intereses</t>
+  </si>
+  <si>
+    <t>campo</t>
+  </si>
+  <si>
+    <t>desc</t>
+  </si>
+  <si>
+    <t>codigo</t>
+  </si>
+  <si>
+    <t>prototipo</t>
+  </si>
+  <si>
+    <t>comentarios</t>
+  </si>
+  <si>
+    <t>reaseguro_proporcional</t>
+  </si>
+  <si>
+    <t>reaseguro_no_proporcional</t>
+  </si>
+  <si>
+    <t>valor_constitucion</t>
+  </si>
+  <si>
+    <t>valor_liberacion</t>
+  </si>
+  <si>
+    <t>indicativo_periodo_movimiento</t>
+  </si>
+  <si>
+    <t>reclasificacion</t>
+  </si>
+  <si>
+    <t>matematica</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -557,8 +1137,50 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Sura Sans"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Sura Sans"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Sura Sans"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Sura Sans"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Sura Sans"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Sura Sans"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Sura Sans"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -571,8 +1193,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -580,18 +1208,85 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -928,8 +1623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FA1C9BF-152D-454C-B2E4-5B164FCAC037}">
   <dimension ref="A1:E69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView showGridLines="0" topLeftCell="A16" zoomScale="144" zoomScaleNormal="144" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -946,88 +1641,91 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" t="s">
         <v>113</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B3" t="s">
         <v>114</v>
       </c>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="C3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>115</v>
       </c>
-      <c r="C3" t="s">
-        <v>115</v>
-      </c>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>116</v>
-      </c>
-      <c r="C4" t="s">
-        <v>120</v>
-      </c>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>117</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
-        <v>118</v>
-      </c>
-      <c r="C6" t="s">
-        <v>121</v>
-      </c>
-      <c r="D6" s="2"/>
+      <c r="B6" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="6" t="s">
         <v>5</v>
       </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -1041,82 +1739,94 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="5" t="s">
         <v>6</v>
       </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>136</v>
+      <c r="D10" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>137</v>
+      <c r="D11" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D12" t="s">
-        <v>141</v>
-      </c>
+      <c r="D12" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="E12" s="6"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="A13" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D13" t="s">
-        <v>140</v>
-      </c>
+      <c r="D13" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="A14" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="6" t="s">
         <v>27</v>
       </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -1152,51 +1862,55 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="A18" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" s="6" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B21" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C21" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" t="s">
-        <v>39</v>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -1204,10 +1918,10 @@
         <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C22" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -1215,13 +1929,10 @@
         <v>13</v>
       </c>
       <c r="B23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C23" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" t="s">
-        <v>142</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -1229,13 +1940,13 @@
         <v>13</v>
       </c>
       <c r="B24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D24" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -1243,13 +1954,13 @@
         <v>13</v>
       </c>
       <c r="B25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D25" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -1257,39 +1968,42 @@
         <v>13</v>
       </c>
       <c r="B26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" t="s">
         <v>21</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>43</v>
       </c>
-      <c r="D26" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
+      <c r="D27" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C27" s="4" t="s">
+      <c r="B28" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="C28" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" t="s">
-        <v>23</v>
-      </c>
-      <c r="C28" t="s">
-        <v>34</v>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -1297,10 +2011,10 @@
         <v>13</v>
       </c>
       <c r="B29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -1308,97 +2022,98 @@
         <v>13</v>
       </c>
       <c r="B30" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D30" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="D31" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="E31" s="5"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D31" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>48</v>
-      </c>
-      <c r="B32" t="s">
-        <v>50</v>
-      </c>
-      <c r="C32" t="s">
-        <v>52</v>
-      </c>
-      <c r="D32" t="s">
-        <v>150</v>
-      </c>
+      <c r="D32" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="E32" s="6"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>48</v>
       </c>
       <c r="B33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D33" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="D34" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="E34" s="5"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D34" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>74</v>
-      </c>
-      <c r="B35" t="s">
-        <v>62</v>
-      </c>
-      <c r="C35" t="s">
-        <v>26</v>
-      </c>
-      <c r="D35" t="s">
-        <v>151</v>
-      </c>
+      <c r="D35" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="E35" s="6"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>74</v>
       </c>
       <c r="B36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C36" t="s">
-        <v>65</v>
+        <v>26</v>
       </c>
       <c r="D36" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -1406,169 +2121,181 @@
         <v>74</v>
       </c>
       <c r="B37" t="s">
+        <v>63</v>
+      </c>
+      <c r="C37" t="s">
+        <v>65</v>
+      </c>
+      <c r="D37" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D37" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+      <c r="D38" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="E38" s="5"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D38" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>66</v>
-      </c>
-      <c r="B39" t="s">
-        <v>69</v>
-      </c>
-      <c r="C39" t="s">
-        <v>70</v>
-      </c>
-      <c r="D39" t="s">
-        <v>155</v>
-      </c>
+      <c r="D39" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="E39" s="6"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>66</v>
       </c>
       <c r="B40" t="s">
+        <v>69</v>
+      </c>
+      <c r="C40" t="s">
+        <v>70</v>
+      </c>
+      <c r="D40" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C41" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D40" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="D41" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="E41" s="5"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C42" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D41" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>75</v>
-      </c>
-      <c r="B42" t="s">
-        <v>77</v>
-      </c>
-      <c r="C42" t="s">
-        <v>79</v>
-      </c>
-      <c r="D42" t="s">
-        <v>157</v>
-      </c>
+      <c r="D42" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="E42" s="6"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>75</v>
       </c>
       <c r="B43" t="s">
-        <v>25</v>
+        <v>77</v>
       </c>
       <c r="C43" t="s">
-        <v>36</v>
+        <v>79</v>
       </c>
       <c r="D43" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="A44" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="E44" s="5"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C45" s="6" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>71</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>81</v>
       </c>
-      <c r="C45" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="5" t="s">
+      <c r="C46" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="B46" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+      <c r="B47" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="D47" s="9"/>
+      <c r="E47" s="10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="B47" t="s">
-        <v>84</v>
-      </c>
-      <c r="C47" t="s">
-        <v>123</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>71</v>
-      </c>
-      <c r="B48" t="s">
-        <v>94</v>
-      </c>
-      <c r="C48" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B48" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="D48" s="9"/>
+      <c r="E48" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>71</v>
       </c>
       <c r="B49" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="C49" t="s">
-        <v>99</v>
+        <v>122</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1576,21 +2303,21 @@
         <v>71</v>
       </c>
       <c r="B50" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C50" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>71</v>
       </c>
       <c r="B51" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C51" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -1601,7 +2328,7 @@
         <v>91</v>
       </c>
       <c r="C52" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -1609,10 +2336,10 @@
         <v>71</v>
       </c>
       <c r="B53" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="C53" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -1620,10 +2347,10 @@
         <v>71</v>
       </c>
       <c r="B54" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C54" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -1631,10 +2358,10 @@
         <v>71</v>
       </c>
       <c r="B55" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C55" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
@@ -1642,32 +2369,32 @@
         <v>71</v>
       </c>
       <c r="B56" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C56" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>71</v>
       </c>
       <c r="B57" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C57" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>71</v>
       </c>
       <c r="B58" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C58" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
@@ -1675,10 +2402,10 @@
         <v>71</v>
       </c>
       <c r="B59" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C59" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -1686,131 +2413,2128 @@
         <v>71</v>
       </c>
       <c r="B60" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C60" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61" s="5" t="s">
+      <c r="A61" t="s">
         <v>71</v>
       </c>
-      <c r="B61" s="5" t="s">
+      <c r="B61" t="s">
+        <v>95</v>
+      </c>
+      <c r="C61" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B62" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C61" s="5" t="s">
+      <c r="C62" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="D62" s="12"/>
+      <c r="E62" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B63" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="C63" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="D63" s="10"/>
+      <c r="E63" s="10" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B64" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="C64" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D64" s="11"/>
+      <c r="E64" s="11" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B65" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="E61" s="5" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="D62" s="5"/>
-      <c r="E62" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="D63" s="5"/>
-      <c r="E63" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>72</v>
-      </c>
-      <c r="B64" t="s">
-        <v>109</v>
-      </c>
-      <c r="C64" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>72</v>
-      </c>
-      <c r="B65" t="s">
-        <v>83</v>
-      </c>
-      <c r="C65" t="s">
-        <v>98</v>
-      </c>
+      <c r="C65" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D65" s="6"/>
+      <c r="E65" s="6"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>72</v>
       </c>
       <c r="B66" t="s">
+        <v>82</v>
+      </c>
+      <c r="C66" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>72</v>
+      </c>
+      <c r="B67" t="s">
         <v>22</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C67" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A67" s="4" t="s">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="B67" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="C67" s="4" t="s">
+      <c r="B68" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C68" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E67" s="5" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
+      <c r="D68" s="9"/>
+      <c r="E68" s="10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
         <v>72</v>
       </c>
-      <c r="B68" t="s">
-        <v>110</v>
-      </c>
-      <c r="C68" t="s">
+      <c r="B69" t="s">
+        <v>109</v>
+      </c>
+      <c r="C69" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A69" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B69" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="C69" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="D69" s="5"/>
-      <c r="E69" s="5" t="s">
-        <v>130</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFD478E0-1E8A-3348-A795-503C066CAB7C}">
+  <dimension ref="A1:E141"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="D68" sqref="D68"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.1640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="54" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>339</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>340</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>342</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" s="16"/>
+    </row>
+    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="16"/>
+    </row>
+    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="16"/>
+    </row>
+    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="16"/>
+    </row>
+    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6" s="19"/>
+      <c r="E6" s="21"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="22"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="21"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="E11" s="21"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="E13" s="21"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D31" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="E31" s="21"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="22" t="s">
+        <v>348</v>
+      </c>
+      <c r="B32" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="D32" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="E32" s="22"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="15" t="s">
+        <v>348</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="21" t="s">
+        <v>348</v>
+      </c>
+      <c r="B34" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D34" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="E34" s="21"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="B35" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="E35" s="22"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B37" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B39" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B40" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D40" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="E40" s="21"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B41" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C41" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D41" s="22" t="s">
+        <v>344</v>
+      </c>
+      <c r="E41" s="22"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B42" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C42" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="B43" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C43" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D43" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="E43" s="21"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="B44" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="C44" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="D44" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="E44" s="22"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B45" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C45" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="D45" s="15" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="B46" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C46" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D46" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="E46" s="21"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B47" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="C47" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="D47" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="E47" s="22"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B48" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="C48" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D48" s="15" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A49" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="B49" s="30" t="s">
+        <v>151</v>
+      </c>
+      <c r="C49" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="D49" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="E49" s="29" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A50" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B50" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C50" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="D50" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="E50" s="29" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B51" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="C51" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="D51" s="15" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B52" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C52" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="D52" s="15" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B53" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="C53" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="D53" s="15" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B54" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="C54" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="D54" s="15" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B55" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C55" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="D55" s="15" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B56" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C56" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="D56" s="15" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B57" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="C57" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="D57" s="15" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B58" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C58" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="D58" s="15" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B59" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C59" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D59" s="15" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A60" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="B60" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C60" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="D60" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="E60" s="29" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A61" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="B61" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="C61" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="D61" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="E61" s="31" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="B62" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="C62" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="D62" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="E62" s="22"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B63" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C63" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="D63" s="15" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B64" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C64" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D64" s="15" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A65" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B65" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="C65" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D65" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="E65" s="29" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B66" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="C66" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D66" s="15" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A67" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B67" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="C67" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="D67" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="E67" s="33"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B68" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="C68" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="D68" s="21" t="s">
+        <v>350</v>
+      </c>
+      <c r="E68" s="21"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="B69" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="C69" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="D69" s="15" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="B70" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C70" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D70" s="15" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="B71" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="C71" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="D71" s="15" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="B72" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="C72" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="D72" s="15" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="B73" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="C73" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="D73" s="15" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="B74" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="C74" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="D74" s="15" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="B75" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="C75" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="D75" s="15" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="B76" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="C76" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="D76" s="15" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="B77" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="C77" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="D77" s="15" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="B78" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="C78" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="D78" s="15" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="B79" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="C79" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="D79" s="15" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="B80" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="C80" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="D80" s="15" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="B81" s="18" t="s">
+        <v>216</v>
+      </c>
+      <c r="C81" s="18" t="s">
+        <v>216</v>
+      </c>
+      <c r="D81" s="15" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="B82" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="C82" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="D82" s="15" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="B83" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="C83" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="D83" s="15" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="B84" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="C84" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="D84" s="15" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="B85" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="C85" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="D85" s="15" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="B86" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="C86" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="D86" s="15" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="B87" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="C87" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="D87" s="15" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="B88" s="18" t="s">
+        <v>230</v>
+      </c>
+      <c r="C88" s="18" t="s">
+        <v>230</v>
+      </c>
+      <c r="D88" s="15" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="B89" s="18" t="s">
+        <v>232</v>
+      </c>
+      <c r="C89" s="18" t="s">
+        <v>232</v>
+      </c>
+      <c r="D89" s="15" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="B90" s="18" t="s">
+        <v>234</v>
+      </c>
+      <c r="C90" s="18" t="s">
+        <v>234</v>
+      </c>
+      <c r="D90" s="15" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="B91" s="18" t="s">
+        <v>236</v>
+      </c>
+      <c r="C91" s="18" t="s">
+        <v>236</v>
+      </c>
+      <c r="D91" s="15" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="B92" s="18" t="s">
+        <v>238</v>
+      </c>
+      <c r="C92" s="18" t="s">
+        <v>238</v>
+      </c>
+      <c r="D92" s="15" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="B93" s="18" t="s">
+        <v>240</v>
+      </c>
+      <c r="C93" s="18" t="s">
+        <v>240</v>
+      </c>
+      <c r="D93" s="15" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="B94" s="20" t="s">
+        <v>242</v>
+      </c>
+      <c r="C94" s="20" t="s">
+        <v>242</v>
+      </c>
+      <c r="D94" s="21" t="s">
+        <v>243</v>
+      </c>
+      <c r="E94" s="21"/>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B95" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="C95" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="D95" s="15" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B96" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="C96" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="D96" s="15" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B97" s="18" t="s">
+        <v>249</v>
+      </c>
+      <c r="C97" s="18" t="s">
+        <v>249</v>
+      </c>
+      <c r="D97" s="15" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B98" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="C98" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="D98" s="15" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B99" s="18" t="s">
+        <v>253</v>
+      </c>
+      <c r="C99" s="18" t="s">
+        <v>253</v>
+      </c>
+      <c r="D99" s="15" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B100" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="C100" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="D100" s="15" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B101" s="18" t="s">
+        <v>257</v>
+      </c>
+      <c r="C101" s="18" t="s">
+        <v>257</v>
+      </c>
+      <c r="D101" s="15" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B102" s="18" t="s">
+        <v>259</v>
+      </c>
+      <c r="C102" s="18" t="s">
+        <v>259</v>
+      </c>
+      <c r="D102" s="15" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B103" s="18" t="s">
+        <v>261</v>
+      </c>
+      <c r="C103" s="18" t="s">
+        <v>261</v>
+      </c>
+      <c r="D103" s="15" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B104" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="C104" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="D104" s="15" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B105" s="18" t="s">
+        <v>265</v>
+      </c>
+      <c r="C105" s="18" t="s">
+        <v>265</v>
+      </c>
+      <c r="D105" s="15" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B106" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="C106" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="D106" s="15" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B107" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="C107" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="D107" s="15" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B108" s="18" t="s">
+        <v>271</v>
+      </c>
+      <c r="C108" s="18" t="s">
+        <v>271</v>
+      </c>
+      <c r="D108" s="15" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B109" s="18" t="s">
+        <v>273</v>
+      </c>
+      <c r="C109" s="18" t="s">
+        <v>273</v>
+      </c>
+      <c r="D109" s="15" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B110" s="18" t="s">
+        <v>275</v>
+      </c>
+      <c r="C110" s="18" t="s">
+        <v>275</v>
+      </c>
+      <c r="D110" s="15" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B111" s="18" t="s">
+        <v>277</v>
+      </c>
+      <c r="C111" s="18" t="s">
+        <v>277</v>
+      </c>
+      <c r="D111" s="15" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B112" s="18" t="s">
+        <v>279</v>
+      </c>
+      <c r="C112" s="18" t="s">
+        <v>279</v>
+      </c>
+      <c r="D112" s="15" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B113" s="18" t="s">
+        <v>281</v>
+      </c>
+      <c r="C113" s="18" t="s">
+        <v>281</v>
+      </c>
+      <c r="D113" s="15" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B114" s="18" t="s">
+        <v>283</v>
+      </c>
+      <c r="C114" s="18" t="s">
+        <v>283</v>
+      </c>
+      <c r="D114" s="15" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B115" s="18" t="s">
+        <v>285</v>
+      </c>
+      <c r="C115" s="18" t="s">
+        <v>285</v>
+      </c>
+      <c r="D115" s="15" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B116" s="18" t="s">
+        <v>287</v>
+      </c>
+      <c r="C116" s="18" t="s">
+        <v>287</v>
+      </c>
+      <c r="D116" s="15" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B117" s="18" t="s">
+        <v>289</v>
+      </c>
+      <c r="C117" s="18" t="s">
+        <v>289</v>
+      </c>
+      <c r="D117" s="15" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B118" s="18" t="s">
+        <v>291</v>
+      </c>
+      <c r="C118" s="18" t="s">
+        <v>291</v>
+      </c>
+      <c r="D118" s="15" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B119" s="18" t="s">
+        <v>293</v>
+      </c>
+      <c r="C119" s="18" t="s">
+        <v>293</v>
+      </c>
+      <c r="D119" s="15" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B120" s="18" t="s">
+        <v>295</v>
+      </c>
+      <c r="C120" s="18" t="s">
+        <v>295</v>
+      </c>
+      <c r="D120" s="15" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B121" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="C121" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="D121" s="15" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B122" s="18" t="s">
+        <v>299</v>
+      </c>
+      <c r="C122" s="18" t="s">
+        <v>299</v>
+      </c>
+      <c r="D122" s="15" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B123" s="18" t="s">
+        <v>301</v>
+      </c>
+      <c r="C123" s="18" t="s">
+        <v>301</v>
+      </c>
+      <c r="D123" s="15" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B124" s="18" t="s">
+        <v>303</v>
+      </c>
+      <c r="C124" s="18" t="s">
+        <v>303</v>
+      </c>
+      <c r="D124" s="15" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B125" s="18" t="s">
+        <v>305</v>
+      </c>
+      <c r="C125" s="18" t="s">
+        <v>305</v>
+      </c>
+      <c r="D125" s="15" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B126" s="18" t="s">
+        <v>307</v>
+      </c>
+      <c r="C126" s="18" t="s">
+        <v>307</v>
+      </c>
+      <c r="D126" s="15" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B127" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="C127" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="D127" s="15" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B128" s="18" t="s">
+        <v>311</v>
+      </c>
+      <c r="C128" s="18" t="s">
+        <v>311</v>
+      </c>
+      <c r="D128" s="15" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B129" s="18" t="s">
+        <v>313</v>
+      </c>
+      <c r="C129" s="18" t="s">
+        <v>313</v>
+      </c>
+      <c r="D129" s="15" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B130" s="18" t="s">
+        <v>315</v>
+      </c>
+      <c r="C130" s="18" t="s">
+        <v>315</v>
+      </c>
+      <c r="D130" s="15" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B131" s="18" t="s">
+        <v>317</v>
+      </c>
+      <c r="C131" s="18" t="s">
+        <v>317</v>
+      </c>
+      <c r="D131" s="15" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B132" s="18" t="s">
+        <v>319</v>
+      </c>
+      <c r="C132" s="18" t="s">
+        <v>319</v>
+      </c>
+      <c r="D132" s="15" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B133" s="18" t="s">
+        <v>321</v>
+      </c>
+      <c r="C133" s="18" t="s">
+        <v>321</v>
+      </c>
+      <c r="D133" s="15" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B134" s="18" t="s">
+        <v>323</v>
+      </c>
+      <c r="C134" s="18" t="s">
+        <v>323</v>
+      </c>
+      <c r="D134" s="15" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B135" s="18" t="s">
+        <v>325</v>
+      </c>
+      <c r="C135" s="18" t="s">
+        <v>325</v>
+      </c>
+      <c r="D135" s="15" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B136" s="18" t="s">
+        <v>327</v>
+      </c>
+      <c r="C136" s="18" t="s">
+        <v>327</v>
+      </c>
+      <c r="D136" s="15" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B137" s="18" t="s">
+        <v>329</v>
+      </c>
+      <c r="C137" s="18" t="s">
+        <v>329</v>
+      </c>
+      <c r="D137" s="15" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B138" s="18" t="s">
+        <v>331</v>
+      </c>
+      <c r="C138" s="18" t="s">
+        <v>331</v>
+      </c>
+      <c r="D138" s="15" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B139" s="18" t="s">
+        <v>333</v>
+      </c>
+      <c r="C139" s="18" t="s">
+        <v>333</v>
+      </c>
+      <c r="D139" s="15" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B140" s="18" t="s">
+        <v>335</v>
+      </c>
+      <c r="C140" s="18" t="s">
+        <v>335</v>
+      </c>
+      <c r="D140" s="15" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B141" s="18" t="s">
+        <v>337</v>
+      </c>
+      <c r="C141" s="18" t="s">
+        <v>337</v>
+      </c>
+      <c r="D141" s="15" t="s">
+        <v>338</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2037,15 +4761,47 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15651A92-013D-43FC-A841-092862588564}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15651A92-013D-43FC-A841-092862588564}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
+    <ds:schemaRef ds:uri="65efab6e-20b9-465e-9733-f0c2ab732419"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F679A37-EAB5-400F-BBD1-820A1C585485}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F679A37-EAB5-400F-BBD1-820A1C585485}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BEEF0C81-D2F9-4EEF-8917-C3A88C6671B0}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BEEF0C81-D2F9-4EEF-8917-C3A88C6671B0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="65efab6e-20b9-465e-9733-f0c2ab732419"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
Ampliar tabla de gastos segun estructura transversal
</commit_message>
<xml_diff>
--- a/prototipo_pcr/inputs/nomenclatura.xlsx
+++ b/prototipo_pcr/inputs/nomenclatura.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebatoec/Library/CloudStorage/OneDrive-SharedLibraries-SegurosSuramericana,S.A/Proyecto féniX - féniX/01 IFRS17/02 Entregables Procesos/05 Reservas/03 PCR CP/03 Tecnología/01 Prototipo/prototipo_pcr/inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://suramericana.sharepoint.com/sites/TraNIFF/Shared Documents/féniX/01 IFRS17/02 Entregables Procesos/05 Reservas/03 PCR CP/03 Tecnología/01 Prototipo/prototipo_pcr/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B14EEF-D4AE-9B47-B041-66E0D9193027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
@@ -4610,6 +4610,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="7ab8c0d4-f18b-4fef-b649-c77d178c2495">
@@ -4618,15 +4627,6 @@
     <TaxCatchAll xmlns="65efab6e-20b9-465e-9733-f0c2ab732419" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4831,26 +4831,26 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BEEF0C81-D2F9-4EEF-8917-C3A88C6671B0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F679A37-EAB5-400F-BBD1-820A1C585485}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
-    <ds:schemaRef ds:uri="65efab6e-20b9-465e-9733-f0c2ab732419"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F679A37-EAB5-400F-BBD1-820A1C585485}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BEEF0C81-D2F9-4EEF-8917-C3A88C6671B0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="65efab6e-20b9-465e-9733-f0c2ab732419"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
feat: Implementar logica de output de cartera
</commit_message>
<xml_diff>
--- a/prototipo_pcr/inputs/nomenclatura.xlsx
+++ b/prototipo_pcr/inputs/nomenclatura.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebatoec/Library/CloudStorage/OneDrive-SharedLibraries-SegurosSuramericana,S.A/Proyecto féniX - féniX/01 IFRS17/01 Archivos de Trabajo/Reservas/02 PCR_CP/03 Tecnología/01 Prototipo/prototipo_pcr/inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebatoec/projects/prototipo_pcr/prototipo_pcr/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82A6D02C-4926-3A45-824B-E293F2BCCE23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C0CF500-3455-764B-8831-2547C19D6F0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1140" windowWidth="27240" windowHeight="16200" activeTab="1" xr2:uid="{B6BBB8B8-7677-D84C-AD85-43B73374E2C3}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17400" activeTab="1" xr2:uid="{B6BBB8B8-7677-D84C-AD85-43B73374E2C3}"/>
   </bookViews>
   <sheets>
     <sheet name="V1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="374">
   <si>
     <t>Campo</t>
   </si>
@@ -570,9 +570,6 @@
     <t>alianza banco</t>
   </si>
   <si>
-    <t>no aplica</t>
-  </si>
-  <si>
     <t>bel</t>
   </si>
   <si>
@@ -1141,6 +1138,27 @@
   </si>
   <si>
     <t>liberacion_deterioro</t>
+  </si>
+  <si>
+    <t>movimiento_cartera</t>
+  </si>
+  <si>
+    <t>Cartera exigible</t>
+  </si>
+  <si>
+    <t>Cartera no exigible</t>
+  </si>
+  <si>
+    <t>CARE</t>
+  </si>
+  <si>
+    <t>CARN</t>
+  </si>
+  <si>
+    <t>cartera_exigible</t>
+  </si>
+  <si>
+    <t>cartera_no_exigible</t>
   </si>
 </sst>
 </file>
@@ -2595,10 +2613,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFD478E0-1E8A-3348-A795-503C066CAB7C}">
-  <dimension ref="A1:E147"/>
+  <dimension ref="A1:E149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -2613,19 +2631,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>339</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="C1" s="13" t="s">
         <v>340</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="13" t="s">
         <v>341</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="14" t="s">
         <v>342</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -2943,13 +2961,13 @@
         <v>13</v>
       </c>
       <c r="B26" s="18" t="s">
+        <v>351</v>
+      </c>
+      <c r="C26" s="18" t="s">
         <v>352</v>
       </c>
-      <c r="C26" s="18" t="s">
-        <v>353</v>
-      </c>
       <c r="D26" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -2957,13 +2975,13 @@
         <v>13</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -2971,13 +2989,13 @@
         <v>13</v>
       </c>
       <c r="B28" s="18" t="s">
+        <v>359</v>
+      </c>
+      <c r="C28" s="18" t="s">
         <v>360</v>
       </c>
-      <c r="C28" s="18" t="s">
-        <v>361</v>
-      </c>
       <c r="D28" s="15" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2985,13 +3003,13 @@
         <v>13</v>
       </c>
       <c r="B29" s="18" t="s">
+        <v>361</v>
+      </c>
+      <c r="C29" s="18" t="s">
         <v>362</v>
       </c>
-      <c r="C29" s="18" t="s">
-        <v>363</v>
-      </c>
       <c r="D29" s="15" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -2999,10 +3017,10 @@
         <v>13</v>
       </c>
       <c r="B30" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="C30" s="18" t="s">
         <v>364</v>
-      </c>
-      <c r="C30" s="18" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -3016,7 +3034,7 @@
         <v>41</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -3030,7 +3048,7 @@
         <v>42</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -3043,6 +3061,9 @@
       <c r="C33" s="18" t="s">
         <v>173</v>
       </c>
+      <c r="D33" s="15" t="s">
+        <v>367</v>
+      </c>
       <c r="E33" s="15" t="s">
         <v>150</v>
       </c>
@@ -3086,7 +3107,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="22" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B37" s="23" t="s">
         <v>49</v>
@@ -3101,7 +3122,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="15" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B38" s="18" t="s">
         <v>50</v>
@@ -3115,7 +3136,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="21" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B39" s="20" t="s">
         <v>25</v>
@@ -3210,7 +3231,7 @@
         <v>36</v>
       </c>
       <c r="D45" s="21" t="s">
-        <v>177</v>
+        <v>137</v>
       </c>
       <c r="E45" s="21"/>
     </row>
@@ -3225,7 +3246,7 @@
         <v>68</v>
       </c>
       <c r="D46" s="22" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E46" s="22"/>
     </row>
@@ -3240,7 +3261,7 @@
         <v>70</v>
       </c>
       <c r="D47" s="15" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -3313,7 +3334,7 @@
         <v>80</v>
       </c>
       <c r="D52" s="15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E52" s="22"/>
     </row>
@@ -3328,7 +3349,7 @@
         <v>96</v>
       </c>
       <c r="D53" s="15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3342,7 +3363,7 @@
         <v>152</v>
       </c>
       <c r="D54" s="15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E54" s="29" t="s">
         <v>153</v>
@@ -3446,7 +3467,7 @@
         <v>97</v>
       </c>
       <c r="D61" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -3460,7 +3481,7 @@
         <v>105</v>
       </c>
       <c r="D62" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -3474,7 +3495,7 @@
         <v>106</v>
       </c>
       <c r="D63" s="15" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -3488,7 +3509,7 @@
         <v>95</v>
       </c>
       <c r="D64" s="15" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3502,7 +3523,7 @@
         <v>107</v>
       </c>
       <c r="D65" s="15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E65" s="29" t="s">
         <v>157</v>
@@ -3513,13 +3534,13 @@
         <v>71</v>
       </c>
       <c r="B66" s="30" t="s">
+        <v>356</v>
+      </c>
+      <c r="C66" s="30" t="s">
         <v>357</v>
       </c>
-      <c r="C66" s="30" t="s">
+      <c r="D66" s="15" t="s">
         <v>358</v>
-      </c>
-      <c r="D66" s="15" t="s">
-        <v>359</v>
       </c>
       <c r="E66" s="29"/>
     </row>
@@ -3551,7 +3572,7 @@
         <v>110</v>
       </c>
       <c r="D68" s="15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E68" s="22"/>
     </row>
@@ -3566,7 +3587,7 @@
         <v>97</v>
       </c>
       <c r="D69" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -3580,24 +3601,21 @@
         <v>32</v>
       </c>
       <c r="D70" s="15" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="15" t="s">
         <v>72</v>
       </c>
       <c r="B71" s="18" t="s">
-        <v>120</v>
+        <v>368</v>
       </c>
       <c r="C71" s="18" t="s">
-        <v>31</v>
+        <v>370</v>
       </c>
       <c r="D71" s="15" t="s">
-        <v>163</v>
-      </c>
-      <c r="E71" s="29" t="s">
-        <v>188</v>
+        <v>372</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -3605,1066 +3623,1097 @@
         <v>72</v>
       </c>
       <c r="B72" s="18" t="s">
-        <v>109</v>
+        <v>369</v>
       </c>
       <c r="C72" s="18" t="s">
-        <v>33</v>
+        <v>371</v>
       </c>
       <c r="D72" s="15" t="s">
-        <v>349</v>
+        <v>373</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A73" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="B73" s="30" t="s">
+      <c r="B73" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="C73" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D73" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="E73" s="29" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B74" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="C74" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D74" s="15" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A75" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B75" s="30" t="s">
         <v>127</v>
       </c>
-      <c r="C73" s="30" t="s">
+      <c r="C75" s="30" t="s">
         <v>127</v>
       </c>
-      <c r="D73" s="15" t="s">
+      <c r="D75" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="E75" s="33"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B76" s="20" t="s">
         <v>189</v>
       </c>
-      <c r="E73" s="33"/>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="B74" s="20" t="s">
+      <c r="C76" s="20" t="s">
         <v>190</v>
       </c>
-      <c r="C74" s="20" t="s">
-        <v>191</v>
-      </c>
-      <c r="D74" s="21" t="s">
-        <v>350</v>
-      </c>
-      <c r="E74" s="21"/>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="15" t="s">
-        <v>192</v>
-      </c>
-      <c r="B75" s="18" t="s">
-        <v>193</v>
-      </c>
-      <c r="C75" s="18" t="s">
-        <v>193</v>
-      </c>
-      <c r="D75" s="15" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="15" t="s">
-        <v>192</v>
-      </c>
-      <c r="B76" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C76" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D76" s="15" t="s">
-        <v>195</v>
-      </c>
+      <c r="D76" s="21" t="s">
+        <v>349</v>
+      </c>
+      <c r="E76" s="21"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="B77" s="18" t="s">
         <v>192</v>
       </c>
-      <c r="B77" s="18" t="s">
-        <v>196</v>
-      </c>
       <c r="C77" s="18" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D77" s="15" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B78" s="18" t="s">
-        <v>198</v>
+        <v>16</v>
       </c>
       <c r="C78" s="18" t="s">
-        <v>198</v>
+        <v>16</v>
       </c>
       <c r="D78" s="15" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B79" s="18" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C79" s="18" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="D79" s="15" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B80" s="18" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C80" s="18" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D80" s="15" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B81" s="18" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="C81" s="18" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="D81" s="15" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B82" s="18" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="C82" s="18" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D82" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B83" s="18" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C83" s="18" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D83" s="15" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B84" s="18" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C84" s="18" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="D84" s="15" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B85" s="18" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C85" s="18" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D85" s="15" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B86" s="18" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="C86" s="18" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="D86" s="15" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B87" s="18" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="C87" s="18" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D87" s="15" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B88" s="18" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C88" s="18" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="D88" s="15" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B89" s="18" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="C89" s="18" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D89" s="15" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B90" s="18" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="C90" s="18" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D90" s="15" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B91" s="18" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C91" s="18" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="D91" s="15" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B92" s="18" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="C92" s="18" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="D92" s="15" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B93" s="18" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C93" s="18" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="D93" s="15" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B94" s="18" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C94" s="18" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="D94" s="15" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B95" s="18" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="C95" s="18" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="D95" s="15" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B96" s="18" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="C96" s="18" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="D96" s="15" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B97" s="18" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="C97" s="18" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="D97" s="15" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B98" s="18" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C98" s="18" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D98" s="15" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B99" s="18" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C99" s="18" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="D99" s="15" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" s="21" t="s">
-        <v>192</v>
-      </c>
-      <c r="B100" s="20" t="s">
-        <v>242</v>
-      </c>
-      <c r="C100" s="20" t="s">
-        <v>242</v>
-      </c>
-      <c r="D100" s="21" t="s">
-        <v>243</v>
-      </c>
-      <c r="E100" s="21"/>
+      <c r="A100" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="B100" s="18" t="s">
+        <v>237</v>
+      </c>
+      <c r="C100" s="18" t="s">
+        <v>237</v>
+      </c>
+      <c r="D100" s="15" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="15" t="s">
-        <v>244</v>
+        <v>191</v>
       </c>
       <c r="B101" s="18" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C101" s="18" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="D101" s="15" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" s="15" t="s">
-        <v>244</v>
-      </c>
-      <c r="B102" s="18" t="s">
-        <v>247</v>
-      </c>
-      <c r="C102" s="18" t="s">
-        <v>247</v>
-      </c>
-      <c r="D102" s="15" t="s">
-        <v>248</v>
-      </c>
+      <c r="A102" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="B102" s="20" t="s">
+        <v>241</v>
+      </c>
+      <c r="C102" s="20" t="s">
+        <v>241</v>
+      </c>
+      <c r="D102" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="E102" s="21"/>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="15" t="s">
+        <v>243</v>
+      </c>
+      <c r="B103" s="18" t="s">
         <v>244</v>
       </c>
-      <c r="B103" s="18" t="s">
-        <v>249</v>
-      </c>
       <c r="C103" s="18" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="D103" s="15" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B104" s="18" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="C104" s="18" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="D104" s="15" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B105" s="18" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="C105" s="18" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="D105" s="15" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B106" s="18" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="C106" s="18" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="D106" s="15" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B107" s="18" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="C107" s="18" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="D107" s="15" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B108" s="18" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="C108" s="18" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="D108" s="15" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B109" s="18" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="C109" s="18" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="D109" s="15" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B110" s="18" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="C110" s="18" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="D110" s="15" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B111" s="18" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="C111" s="18" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="D111" s="15" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B112" s="18" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="C112" s="18" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="D112" s="15" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B113" s="18" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="C113" s="18" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="D113" s="15" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B114" s="18" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="C114" s="18" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="D114" s="15" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B115" s="18" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="C115" s="18" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="D115" s="15" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B116" s="18" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="C116" s="18" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="D116" s="15" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B117" s="18" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C117" s="18" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="D117" s="15" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B118" s="18" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="C118" s="18" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="D118" s="15" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B119" s="18" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="C119" s="18" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="D119" s="15" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B120" s="18" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="C120" s="18" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="D120" s="15" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B121" s="18" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="C121" s="18" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D121" s="15" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B122" s="18" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="C122" s="18" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="D122" s="15" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B123" s="18" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="C123" s="18" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="D123" s="15" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B124" s="18" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="C124" s="18" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="D124" s="15" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B125" s="18" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="C125" s="18" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="D125" s="15" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B126" s="18" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C126" s="18" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="D126" s="15" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B127" s="18" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="C127" s="18" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="D127" s="15" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B128" s="18" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="C128" s="18" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="D128" s="15" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B129" s="18" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="C129" s="18" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="D129" s="15" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B130" s="18" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="C130" s="18" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="D130" s="15" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B131" s="18" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C131" s="18" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="D131" s="15" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B132" s="18" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="C132" s="18" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="D132" s="15" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B133" s="18" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="C133" s="18" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="D133" s="15" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B134" s="18" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="C134" s="18" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="D134" s="15" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B135" s="18" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="C135" s="18" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="D135" s="15" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B136" s="18" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="C136" s="18" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="D136" s="15" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B137" s="18" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="C137" s="18" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="D137" s="15" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B138" s="18" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="C138" s="18" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="D138" s="15" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B139" s="18" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="C139" s="18" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="D139" s="15" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B140" s="18" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="C140" s="18" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="D140" s="15" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B141" s="18" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="C141" s="18" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="D141" s="15" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B142" s="18" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="C142" s="18" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="D142" s="15" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B143" s="18" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="C143" s="18" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="D143" s="15" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B144" s="18" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="C144" s="18" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="D144" s="15" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B145" s="18" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="C145" s="18" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="D145" s="15" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B146" s="18" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="C146" s="18" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="D146" s="15" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B147" s="18" t="s">
+        <v>332</v>
+      </c>
+      <c r="C147" s="18" t="s">
+        <v>332</v>
+      </c>
+      <c r="D147" s="15" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" s="15" t="s">
+        <v>243</v>
+      </c>
+      <c r="B148" s="18" t="s">
+        <v>334</v>
+      </c>
+      <c r="C148" s="18" t="s">
+        <v>334</v>
+      </c>
+      <c r="D148" s="15" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" s="15" t="s">
+        <v>243</v>
+      </c>
+      <c r="B149" s="18" t="s">
+        <v>336</v>
+      </c>
+      <c r="C149" s="18" t="s">
+        <v>336</v>
+      </c>
+      <c r="D149" s="15" t="s">
         <v>337</v>
-      </c>
-      <c r="C147" s="18" t="s">
-        <v>337</v>
-      </c>
-      <c r="D147" s="15" t="s">
-        <v>338</v>
       </c>
     </row>
   </sheetData>
@@ -4874,6 +4923,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="7ab8c0d4-f18b-4fef-b649-c77d178c2495">
@@ -4882,15 +4940,6 @@
     <TaxCatchAll xmlns="65efab6e-20b9-465e-9733-f0c2ab732419" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4913,6 +4962,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F679A37-EAB5-400F-BBD1-820A1C585485}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BEEF0C81-D2F9-4EEF-8917-C3A88C6671B0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -4929,14 +4986,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F679A37-EAB5-400F-BBD1-820A1C585485}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{3c0bd4fe-1111-4d13-8e0c-7c33b9eb7581}" enabled="0" method="" siteId="{3c0bd4fe-1111-4d13-8e0c-7c33b9eb7581}" removed="1"/>

</xml_diff>

<commit_message>
fix: Corregir transición e incluirla en el cruce bt
</commit_message>
<xml_diff>
--- a/prototipo_pcr/inputs/nomenclatura.xlsx
+++ b/prototipo_pcr/inputs/nomenclatura.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebatoec/projects/prototipo_pcr/prototipo_pcr/inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samuarta\Proyectos\prototipo-pcr\prototipo_pcr\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F9F99E-2D4C-6144-A58B-3E2DCE2A11B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC62F7EB-9202-4576-8306-599B49752775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17400" activeTab="1" xr2:uid="{B6BBB8B8-7677-D84C-AD85-43B73374E2C3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{B6BBB8B8-7677-D84C-AD85-43B73374E2C3}"/>
   </bookViews>
   <sheets>
     <sheet name="V1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="382">
   <si>
     <t>Campo</t>
   </si>
@@ -1168,6 +1168,21 @@
   </si>
   <si>
     <t>costo_contrato</t>
+  </si>
+  <si>
+    <t>transicion</t>
+  </si>
+  <si>
+    <t>Si</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Es transición</t>
+  </si>
+  <si>
+    <t>No es transición</t>
   </si>
 </sst>
 </file>
@@ -1705,7 +1720,7 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
@@ -1714,7 +1729,7 @@
     <col min="5" max="5" width="49.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1731,7 +1746,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -1743,7 +1758,7 @@
       </c>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -1755,7 +1770,7 @@
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -1767,7 +1782,7 @@
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -1779,7 +1794,7 @@
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
@@ -1792,7 +1807,7 @@
       <c r="D6" s="4"/>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
@@ -1805,7 +1820,7 @@
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -1816,7 +1831,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
         <v>1</v>
       </c>
@@ -1829,7 +1844,7 @@
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" s="6" t="s">
         <v>10</v>
       </c>
@@ -1846,7 +1861,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
@@ -1863,7 +1878,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" s="6" t="s">
         <v>55</v>
       </c>
@@ -1878,7 +1893,7 @@
       </c>
       <c r="E12" s="6"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" s="5" t="s">
         <v>55</v>
       </c>
@@ -1893,7 +1908,7 @@
       </c>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" s="6" t="s">
         <v>73</v>
       </c>
@@ -1906,7 +1921,7 @@
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>73</v>
       </c>
@@ -1917,7 +1932,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>73</v>
       </c>
@@ -1928,7 +1943,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>73</v>
       </c>
@@ -1939,7 +1954,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18" s="9" t="s">
         <v>73</v>
       </c>
@@ -1950,7 +1965,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A19" s="5" t="s">
         <v>73</v>
       </c>
@@ -1963,7 +1978,7 @@
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A20" s="6" t="s">
         <v>13</v>
       </c>
@@ -1976,7 +1991,7 @@
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A21" s="9" t="s">
         <v>13</v>
       </c>
@@ -1991,7 +2006,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -2002,7 +2017,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -2013,7 +2028,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -2027,7 +2042,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -2041,7 +2056,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -2055,7 +2070,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -2069,7 +2084,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A28" s="9" t="s">
         <v>13</v>
       </c>
@@ -2084,7 +2099,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>13</v>
       </c>
@@ -2095,7 +2110,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>13</v>
       </c>
@@ -2106,7 +2121,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A31" s="5" t="s">
         <v>13</v>
       </c>
@@ -2121,7 +2136,7 @@
       </c>
       <c r="E31" s="5"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A32" s="6" t="s">
         <v>48</v>
       </c>
@@ -2136,7 +2151,7 @@
       </c>
       <c r="E32" s="6"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>48</v>
       </c>
@@ -2150,7 +2165,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A34" s="5" t="s">
         <v>48</v>
       </c>
@@ -2165,7 +2180,7 @@
       </c>
       <c r="E34" s="5"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A35" s="6" t="s">
         <v>74</v>
       </c>
@@ -2180,7 +2195,7 @@
       </c>
       <c r="E35" s="6"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>74</v>
       </c>
@@ -2194,7 +2209,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>74</v>
       </c>
@@ -2208,7 +2223,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A38" s="5" t="s">
         <v>74</v>
       </c>
@@ -2223,7 +2238,7 @@
       </c>
       <c r="E38" s="5"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A39" s="6" t="s">
         <v>66</v>
       </c>
@@ -2238,7 +2253,7 @@
       </c>
       <c r="E39" s="6"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>66</v>
       </c>
@@ -2252,7 +2267,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A41" s="5" t="s">
         <v>66</v>
       </c>
@@ -2267,7 +2282,7 @@
       </c>
       <c r="E41" s="5"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A42" s="6" t="s">
         <v>75</v>
       </c>
@@ -2282,7 +2297,7 @@
       </c>
       <c r="E42" s="6"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>75</v>
       </c>
@@ -2296,7 +2311,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A44" s="5" t="s">
         <v>75</v>
       </c>
@@ -2311,7 +2326,7 @@
       </c>
       <c r="E44" s="5"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A45" s="6" t="s">
         <v>71</v>
       </c>
@@ -2324,7 +2339,7 @@
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
         <v>71</v>
       </c>
@@ -2335,7 +2350,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A47" s="10" t="s">
         <v>71</v>
       </c>
@@ -2350,7 +2365,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A48" s="9" t="s">
         <v>71</v>
       </c>
@@ -2365,7 +2380,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
         <v>71</v>
       </c>
@@ -2376,7 +2391,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
         <v>71</v>
       </c>
@@ -2387,7 +2402,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
         <v>71</v>
       </c>
@@ -2398,7 +2413,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
         <v>71</v>
       </c>
@@ -2409,7 +2424,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
         <v>71</v>
       </c>
@@ -2420,7 +2435,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A54" t="s">
         <v>71</v>
       </c>
@@ -2431,7 +2446,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A55" t="s">
         <v>71</v>
       </c>
@@ -2442,7 +2457,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
         <v>71</v>
       </c>
@@ -2453,7 +2468,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A57" t="s">
         <v>71</v>
       </c>
@@ -2464,7 +2479,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A58" t="s">
         <v>71</v>
       </c>
@@ -2475,7 +2490,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A59" t="s">
         <v>71</v>
       </c>
@@ -2486,7 +2501,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A60" t="s">
         <v>71</v>
       </c>
@@ -2497,7 +2512,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A61" t="s">
         <v>71</v>
       </c>
@@ -2508,7 +2523,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A62" s="12" t="s">
         <v>71</v>
       </c>
@@ -2523,7 +2538,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A63" s="10" t="s">
         <v>71</v>
       </c>
@@ -2538,7 +2553,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A64" s="11" t="s">
         <v>71</v>
       </c>
@@ -2553,7 +2568,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A65" s="6" t="s">
         <v>72</v>
       </c>
@@ -2566,7 +2581,7 @@
       <c r="D65" s="6"/>
       <c r="E65" s="6"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A66" t="s">
         <v>72</v>
       </c>
@@ -2577,7 +2592,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A67" t="s">
         <v>72</v>
       </c>
@@ -2588,7 +2603,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A68" s="9" t="s">
         <v>72</v>
       </c>
@@ -2603,7 +2618,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A69" t="s">
         <v>72</v>
       </c>
@@ -2622,13 +2637,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFD478E0-1E8A-3348-A795-503C066CAB7C}">
-  <dimension ref="A1:E150"/>
+  <dimension ref="A1:E152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+    <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
+      <selection activeCell="B154" sqref="B154"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="29.5" style="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.5" style="18" bestFit="1" customWidth="1"/>
@@ -2638,7 +2653,7 @@
     <col min="6" max="16384" width="10.83203125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="16.5" x14ac:dyDescent="0.4">
       <c r="A1" s="13" t="s">
         <v>338</v>
       </c>
@@ -2655,7 +2670,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.4">
       <c r="A2" s="16" t="s">
         <v>8</v>
       </c>
@@ -2667,7 +2682,7 @@
       </c>
       <c r="D2" s="16"/>
     </row>
-    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.4">
       <c r="A3" s="16" t="s">
         <v>8</v>
       </c>
@@ -2679,7 +2694,7 @@
       </c>
       <c r="D3" s="16"/>
     </row>
-    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.4">
       <c r="A4" s="16" t="s">
         <v>8</v>
       </c>
@@ -2691,7 +2706,7 @@
       </c>
       <c r="D4" s="16"/>
     </row>
-    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.4">
       <c r="A5" s="16" t="s">
         <v>8</v>
       </c>
@@ -2703,7 +2718,7 @@
       </c>
       <c r="D5" s="16"/>
     </row>
-    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.4">
       <c r="A6" s="19" t="s">
         <v>8</v>
       </c>
@@ -2716,7 +2731,7 @@
       <c r="D6" s="19"/>
       <c r="E6" s="21"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7" s="22" t="s">
         <v>1</v>
       </c>
@@ -2731,7 +2746,7 @@
       </c>
       <c r="E7" s="22"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8" s="15" t="s">
         <v>1</v>
       </c>
@@ -2745,7 +2760,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" s="21" t="s">
         <v>1</v>
       </c>
@@ -2760,7 +2775,7 @@
       </c>
       <c r="E9" s="21"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" s="22" t="s">
         <v>10</v>
       </c>
@@ -2774,7 +2789,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" s="21" t="s">
         <v>10</v>
       </c>
@@ -2789,7 +2804,7 @@
       </c>
       <c r="E11" s="21"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" s="22" t="s">
         <v>55</v>
       </c>
@@ -2803,7 +2818,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" s="21" t="s">
         <v>55</v>
       </c>
@@ -2818,7 +2833,7 @@
       </c>
       <c r="E13" s="21"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" s="22" t="s">
         <v>73</v>
       </c>
@@ -2831,7 +2846,7 @@
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15" s="15" t="s">
         <v>73</v>
       </c>
@@ -2842,7 +2857,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16" s="15" t="s">
         <v>73</v>
       </c>
@@ -2853,7 +2868,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17" s="15" t="s">
         <v>73</v>
       </c>
@@ -2864,7 +2879,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18" s="15" t="s">
         <v>73</v>
       </c>
@@ -2875,7 +2890,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A19" s="21" t="s">
         <v>73</v>
       </c>
@@ -2888,7 +2903,7 @@
       <c r="D19" s="21"/>
       <c r="E19" s="21"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A20" s="22" t="s">
         <v>13</v>
       </c>
@@ -2901,7 +2916,7 @@
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A21" s="15" t="s">
         <v>13</v>
       </c>
@@ -2915,7 +2930,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A22" s="15" t="s">
         <v>13</v>
       </c>
@@ -2929,7 +2944,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A23" s="15" t="s">
         <v>13</v>
       </c>
@@ -2940,7 +2955,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A24" s="15" t="s">
         <v>13</v>
       </c>
@@ -2951,7 +2966,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A25" s="15" t="s">
         <v>13</v>
       </c>
@@ -2965,7 +2980,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A26" s="15" t="s">
         <v>13</v>
       </c>
@@ -2979,7 +2994,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A27" s="15" t="s">
         <v>13</v>
       </c>
@@ -2993,7 +3008,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A28" s="15" t="s">
         <v>13</v>
       </c>
@@ -3007,7 +3022,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A29" s="15" t="s">
         <v>13</v>
       </c>
@@ -3021,7 +3036,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A30" s="15" t="s">
         <v>13</v>
       </c>
@@ -3032,7 +3047,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A31" s="15" t="s">
         <v>13</v>
       </c>
@@ -3046,7 +3061,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A32" s="15" t="s">
         <v>13</v>
       </c>
@@ -3060,7 +3075,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A33" s="15" t="s">
         <v>13</v>
       </c>
@@ -3077,7 +3092,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A34" s="15" t="s">
         <v>13</v>
       </c>
@@ -3088,7 +3103,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A35" s="15" t="s">
         <v>13</v>
       </c>
@@ -3099,7 +3114,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A36" s="21" t="s">
         <v>13</v>
       </c>
@@ -3114,7 +3129,7 @@
       </c>
       <c r="E36" s="21"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A37" s="22" t="s">
         <v>347</v>
       </c>
@@ -3129,7 +3144,7 @@
       </c>
       <c r="E37" s="22"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A38" s="15" t="s">
         <v>347</v>
       </c>
@@ -3143,7 +3158,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A39" s="21" t="s">
         <v>347</v>
       </c>
@@ -3158,7 +3173,7 @@
       </c>
       <c r="E39" s="21"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A40" s="22" t="s">
         <v>74</v>
       </c>
@@ -3173,7 +3188,7 @@
       </c>
       <c r="E40" s="22"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A41" s="15" t="s">
         <v>74</v>
       </c>
@@ -3187,7 +3202,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A42" s="15" t="s">
         <v>74</v>
       </c>
@@ -3201,7 +3216,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A43" s="15" t="s">
         <v>74</v>
       </c>
@@ -3215,7 +3230,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A44" s="15" t="s">
         <v>74</v>
       </c>
@@ -3229,7 +3244,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A45" s="15" t="s">
         <v>74</v>
       </c>
@@ -3244,7 +3259,7 @@
       </c>
       <c r="E45" s="21"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A46" s="22" t="s">
         <v>66</v>
       </c>
@@ -3259,7 +3274,7 @@
       </c>
       <c r="E46" s="22"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A47" s="15" t="s">
         <v>66</v>
       </c>
@@ -3273,7 +3288,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A48" s="21" t="s">
         <v>66</v>
       </c>
@@ -3288,7 +3303,7 @@
       </c>
       <c r="E48" s="21"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A49" s="22" t="s">
         <v>75</v>
       </c>
@@ -3303,7 +3318,7 @@
       </c>
       <c r="E49" s="22"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A50" s="15" t="s">
         <v>75</v>
       </c>
@@ -3317,7 +3332,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A51" s="21" t="s">
         <v>75</v>
       </c>
@@ -3332,7 +3347,7 @@
       </c>
       <c r="E51" s="21"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A52" s="22" t="s">
         <v>71</v>
       </c>
@@ -3347,7 +3362,7 @@
       </c>
       <c r="E52" s="22"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A53" s="15" t="s">
         <v>71</v>
       </c>
@@ -3361,7 +3376,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="16.5" x14ac:dyDescent="0.4">
       <c r="A54" s="29" t="s">
         <v>71</v>
       </c>
@@ -3378,7 +3393,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" ht="16.5" x14ac:dyDescent="0.4">
       <c r="A55" s="15" t="s">
         <v>71</v>
       </c>
@@ -3395,7 +3410,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" ht="16.5" x14ac:dyDescent="0.4">
       <c r="A56" s="15" t="s">
         <v>71</v>
       </c>
@@ -3410,7 +3425,7 @@
       </c>
       <c r="E56" s="29"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A57" s="15" t="s">
         <v>71</v>
       </c>
@@ -3424,7 +3439,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A58" s="15" t="s">
         <v>71</v>
       </c>
@@ -3438,7 +3453,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A59" s="15" t="s">
         <v>71</v>
       </c>
@@ -3452,7 +3467,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A60" s="15" t="s">
         <v>71</v>
       </c>
@@ -3466,7 +3481,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A61" s="15" t="s">
         <v>71</v>
       </c>
@@ -3480,7 +3495,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A62" s="15" t="s">
         <v>71</v>
       </c>
@@ -3494,7 +3509,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A63" s="15" t="s">
         <v>71</v>
       </c>
@@ -3508,7 +3523,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A64" s="15" t="s">
         <v>71</v>
       </c>
@@ -3522,7 +3537,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A65" s="15" t="s">
         <v>71</v>
       </c>
@@ -3536,7 +3551,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" ht="16.5" x14ac:dyDescent="0.4">
       <c r="A66" s="29" t="s">
         <v>71</v>
       </c>
@@ -3553,7 +3568,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" ht="16.5" x14ac:dyDescent="0.4">
       <c r="A67" s="29" t="s">
         <v>71</v>
       </c>
@@ -3568,7 +3583,7 @@
       </c>
       <c r="E67" s="29"/>
     </row>
-    <row r="68" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" ht="16.5" x14ac:dyDescent="0.4">
       <c r="A68" s="31" t="s">
         <v>71</v>
       </c>
@@ -3585,7 +3600,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A69" s="22" t="s">
         <v>72</v>
       </c>
@@ -3600,7 +3615,7 @@
       </c>
       <c r="E69" s="22"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A70" s="15" t="s">
         <v>72</v>
       </c>
@@ -3614,7 +3629,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A71" s="15" t="s">
         <v>72</v>
       </c>
@@ -3628,7 +3643,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A72" s="15" t="s">
         <v>72</v>
       </c>
@@ -3642,7 +3657,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A73" s="15" t="s">
         <v>72</v>
       </c>
@@ -3656,7 +3671,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" ht="16.5" x14ac:dyDescent="0.4">
       <c r="A74" s="15" t="s">
         <v>72</v>
       </c>
@@ -3673,7 +3688,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A75" s="15" t="s">
         <v>72</v>
       </c>
@@ -3687,7 +3702,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" ht="16.5" x14ac:dyDescent="0.4">
       <c r="A76" s="15" t="s">
         <v>72</v>
       </c>
@@ -3702,7 +3717,7 @@
       </c>
       <c r="E76" s="33"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A77" s="21" t="s">
         <v>72</v>
       </c>
@@ -3717,7 +3732,7 @@
       </c>
       <c r="E77" s="21"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A78" s="15" t="s">
         <v>191</v>
       </c>
@@ -3731,7 +3746,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A79" s="15" t="s">
         <v>191</v>
       </c>
@@ -3745,7 +3760,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A80" s="15" t="s">
         <v>191</v>
       </c>
@@ -3759,7 +3774,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A81" s="15" t="s">
         <v>191</v>
       </c>
@@ -3773,7 +3788,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A82" s="15" t="s">
         <v>191</v>
       </c>
@@ -3787,7 +3802,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A83" s="15" t="s">
         <v>191</v>
       </c>
@@ -3801,7 +3816,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A84" s="15" t="s">
         <v>191</v>
       </c>
@@ -3815,7 +3830,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A85" s="15" t="s">
         <v>191</v>
       </c>
@@ -3829,7 +3844,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A86" s="15" t="s">
         <v>191</v>
       </c>
@@ -3843,7 +3858,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A87" s="15" t="s">
         <v>191</v>
       </c>
@@ -3857,7 +3872,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A88" s="15" t="s">
         <v>191</v>
       </c>
@@ -3871,7 +3886,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A89" s="15" t="s">
         <v>191</v>
       </c>
@@ -3885,7 +3900,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A90" s="15" t="s">
         <v>191</v>
       </c>
@@ -3899,7 +3914,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A91" s="15" t="s">
         <v>191</v>
       </c>
@@ -3913,7 +3928,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A92" s="15" t="s">
         <v>191</v>
       </c>
@@ -3927,7 +3942,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A93" s="15" t="s">
         <v>191</v>
       </c>
@@ -3941,7 +3956,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A94" s="15" t="s">
         <v>191</v>
       </c>
@@ -3955,7 +3970,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A95" s="15" t="s">
         <v>191</v>
       </c>
@@ -3969,7 +3984,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A96" s="15" t="s">
         <v>191</v>
       </c>
@@ -3983,7 +3998,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A97" s="15" t="s">
         <v>191</v>
       </c>
@@ -3997,7 +4012,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A98" s="15" t="s">
         <v>191</v>
       </c>
@@ -4011,7 +4026,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A99" s="15" t="s">
         <v>191</v>
       </c>
@@ -4025,7 +4040,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A100" s="15" t="s">
         <v>191</v>
       </c>
@@ -4039,7 +4054,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A101" s="15" t="s">
         <v>191</v>
       </c>
@@ -4053,7 +4068,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A102" s="15" t="s">
         <v>191</v>
       </c>
@@ -4067,7 +4082,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A103" s="21" t="s">
         <v>191</v>
       </c>
@@ -4082,7 +4097,7 @@
       </c>
       <c r="E103" s="21"/>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A104" s="15" t="s">
         <v>243</v>
       </c>
@@ -4096,7 +4111,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A105" s="15" t="s">
         <v>243</v>
       </c>
@@ -4110,7 +4125,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A106" s="15" t="s">
         <v>243</v>
       </c>
@@ -4124,7 +4139,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A107" s="15" t="s">
         <v>243</v>
       </c>
@@ -4138,7 +4153,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A108" s="15" t="s">
         <v>243</v>
       </c>
@@ -4152,7 +4167,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A109" s="15" t="s">
         <v>243</v>
       </c>
@@ -4166,7 +4181,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A110" s="15" t="s">
         <v>243</v>
       </c>
@@ -4180,7 +4195,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A111" s="15" t="s">
         <v>243</v>
       </c>
@@ -4194,7 +4209,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A112" s="15" t="s">
         <v>243</v>
       </c>
@@ -4208,7 +4223,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A113" s="15" t="s">
         <v>243</v>
       </c>
@@ -4222,7 +4237,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A114" s="15" t="s">
         <v>243</v>
       </c>
@@ -4236,7 +4251,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A115" s="15" t="s">
         <v>243</v>
       </c>
@@ -4250,7 +4265,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A116" s="15" t="s">
         <v>243</v>
       </c>
@@ -4264,7 +4279,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A117" s="15" t="s">
         <v>243</v>
       </c>
@@ -4278,7 +4293,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A118" s="15" t="s">
         <v>243</v>
       </c>
@@ -4292,7 +4307,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A119" s="15" t="s">
         <v>243</v>
       </c>
@@ -4306,7 +4321,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A120" s="15" t="s">
         <v>243</v>
       </c>
@@ -4320,7 +4335,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A121" s="15" t="s">
         <v>243</v>
       </c>
@@ -4334,7 +4349,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A122" s="15" t="s">
         <v>243</v>
       </c>
@@ -4348,7 +4363,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A123" s="15" t="s">
         <v>243</v>
       </c>
@@ -4362,7 +4377,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A124" s="15" t="s">
         <v>243</v>
       </c>
@@ -4376,7 +4391,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A125" s="15" t="s">
         <v>243</v>
       </c>
@@ -4390,7 +4405,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A126" s="15" t="s">
         <v>243</v>
       </c>
@@ -4404,7 +4419,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A127" s="15" t="s">
         <v>243</v>
       </c>
@@ -4418,7 +4433,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A128" s="15" t="s">
         <v>243</v>
       </c>
@@ -4432,7 +4447,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A129" s="15" t="s">
         <v>243</v>
       </c>
@@ -4446,7 +4461,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A130" s="15" t="s">
         <v>243</v>
       </c>
@@ -4460,7 +4475,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A131" s="15" t="s">
         <v>243</v>
       </c>
@@ -4474,7 +4489,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A132" s="15" t="s">
         <v>243</v>
       </c>
@@ -4488,7 +4503,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A133" s="15" t="s">
         <v>243</v>
       </c>
@@ -4502,7 +4517,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A134" s="15" t="s">
         <v>243</v>
       </c>
@@ -4516,7 +4531,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A135" s="15" t="s">
         <v>243</v>
       </c>
@@ -4530,7 +4545,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A136" s="15" t="s">
         <v>243</v>
       </c>
@@ -4544,7 +4559,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A137" s="15" t="s">
         <v>243</v>
       </c>
@@ -4558,7 +4573,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A138" s="15" t="s">
         <v>243</v>
       </c>
@@ -4572,7 +4587,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A139" s="15" t="s">
         <v>243</v>
       </c>
@@ -4586,7 +4601,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A140" s="15" t="s">
         <v>243</v>
       </c>
@@ -4600,7 +4615,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A141" s="15" t="s">
         <v>243</v>
       </c>
@@ -4614,7 +4629,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A142" s="15" t="s">
         <v>243</v>
       </c>
@@ -4628,7 +4643,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A143" s="15" t="s">
         <v>243</v>
       </c>
@@ -4642,7 +4657,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A144" s="15" t="s">
         <v>243</v>
       </c>
@@ -4656,7 +4671,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A145" s="15" t="s">
         <v>243</v>
       </c>
@@ -4670,7 +4685,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A146" s="15" t="s">
         <v>243</v>
       </c>
@@ -4684,7 +4699,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A147" s="15" t="s">
         <v>243</v>
       </c>
@@ -4698,7 +4713,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A148" s="15" t="s">
         <v>243</v>
       </c>
@@ -4712,7 +4727,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A149" s="15" t="s">
         <v>243</v>
       </c>
@@ -4726,26 +4741,65 @@
         <v>335</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" s="15" t="s">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A150" s="21" t="s">
         <v>243</v>
       </c>
-      <c r="B150" s="18" t="s">
+      <c r="B150" s="20" t="s">
         <v>336</v>
       </c>
-      <c r="C150" s="18" t="s">
+      <c r="C150" s="20" t="s">
         <v>336</v>
       </c>
-      <c r="D150" s="15" t="s">
+      <c r="D150" s="21" t="s">
         <v>337</v>
+      </c>
+      <c r="E150" s="21"/>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A151" s="15" t="s">
+        <v>377</v>
+      </c>
+      <c r="B151" s="18" t="s">
+        <v>380</v>
+      </c>
+      <c r="C151" s="18" t="s">
+        <v>378</v>
+      </c>
+      <c r="D151" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A152" s="15" t="s">
+        <v>377</v>
+      </c>
+      <c r="B152" s="18" t="s">
+        <v>381</v>
+      </c>
+      <c r="C152" s="18" t="s">
+        <v>379</v>
+      </c>
+      <c r="D152" s="15">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="7ab8c0d4-f18b-4fef-b649-c77d178c2495">
@@ -4754,15 +4808,6 @@
     <TaxCatchAll xmlns="65efab6e-20b9-465e-9733-f0c2ab732419" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4967,6 +5012,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F679A37-EAB5-400F-BBD1-820A1C585485}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BEEF0C81-D2F9-4EEF-8917-C3A88C6671B0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -4979,14 +5032,6 @@
     <ds:schemaRef ds:uri="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F679A37-EAB5-400F-BBD1-820A1C585485}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
feat: Implementar comparación Tecnología/Prototipo
</commit_message>
<xml_diff>
--- a/prototipo_pcr/inputs/nomenclatura.xlsx
+++ b/prototipo_pcr/inputs/nomenclatura.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samuarta\Proyectos\prototipo-pcr\prototipo_pcr\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC62F7EB-9202-4576-8306-599B49752775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EB65200-B037-47B7-85F3-C51DD2FACE12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{B6BBB8B8-7677-D84C-AD85-43B73374E2C3}"/>
   </bookViews>
@@ -1173,16 +1173,16 @@
     <t>transicion</t>
   </si>
   <si>
-    <t>Si</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>Es transición</t>
   </si>
   <si>
     <t>No es transición</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>NO</t>
   </si>
 </sst>
 </file>
@@ -2640,7 +2640,7 @@
   <dimension ref="A1:E152"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
-      <selection activeCell="B154" sqref="B154"/>
+      <selection activeCell="C151" sqref="C151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
@@ -4761,10 +4761,10 @@
         <v>377</v>
       </c>
       <c r="B151" s="18" t="s">
+        <v>378</v>
+      </c>
+      <c r="C151" s="18" t="s">
         <v>380</v>
-      </c>
-      <c r="C151" s="18" t="s">
-        <v>378</v>
       </c>
       <c r="D151" s="15">
         <v>1</v>
@@ -4775,10 +4775,10 @@
         <v>377</v>
       </c>
       <c r="B152" s="18" t="s">
+        <v>379</v>
+      </c>
+      <c r="C152" s="18" t="s">
         <v>381</v>
-      </c>
-      <c r="C152" s="18" t="s">
-        <v>379</v>
       </c>
       <c r="D152" s="15">
         <v>0</v>

</xml_diff>